<commit_message>
configurado parte do gráfico e melhorado código
</commit_message>
<xml_diff>
--- a/planilhas/Solar-evolution-chart.xlsx
+++ b/planilhas/Solar-evolution-chart.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ferreira/Documents/Projetos Flutter/absolar/planilhas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FD5C74B-A92B-664E-8425-9ACD0F5E352B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA69AAAA-79EC-6A47-98E0-2C0A24B17E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15500" xr2:uid="{E906F46E-C93F-CE41-A4C1-065F97F16B82}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>column1</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -137,8 +140,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -261,12 +264,11 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="5" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -276,7 +278,7 @@
     <xf numFmtId="3" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="5" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,19 +609,19 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="10.83203125" style="2"/>
-    <col min="11" max="11" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,40 +657,40 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>6.8</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>11.25</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>16.82</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>27.740000000000002</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>29.410000000000004</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>968.11</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>1824.52</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>2475.4299999999998</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>3093.0699999999997</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <v>4632.2476100000003</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="3">
         <v>5927.01</v>
       </c>
     </row>
@@ -696,37 +698,37 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.46722000000000002</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1.393</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>3.9870000000000001</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>13.28</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>61.935000000000002</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>190</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>591</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>2134</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="8">
         <v>4923.4855100019413</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="9">
         <v>9185.453090006682</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="10">
         <v>12727.056520007489</v>
       </c>
     </row>
@@ -734,47 +736,47 @@
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <f>B2+B3</f>
         <v>7.26722</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="11">
         <f t="shared" ref="C4:L4" si="0">C2+C3</f>
         <v>12.643000000000001</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <f t="shared" si="0"/>
         <v>20.807000000000002</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <f t="shared" si="0"/>
         <v>41.02</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <f t="shared" si="0"/>
         <v>91.344999999999999</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <f t="shared" si="0"/>
         <v>1158.1100000000001</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="11">
         <f t="shared" si="0"/>
         <v>2415.52</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <f t="shared" si="0"/>
         <v>4609.43</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="11">
         <f t="shared" si="0"/>
         <v>8016.555510001941</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <f t="shared" si="0"/>
         <v>13817.700700006682</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="11">
         <f t="shared" si="0"/>
         <v>18654.066520007487</v>
       </c>

</xml_diff>